<commit_message>
Final upload for part 2
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quant\Documents\Uni Docs\Griffith Uni Docs\2810ICT\part 2 documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE4AFBA2-CD0D-41E6-A7B3-60742577B0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415549D1-EB25-427A-9299-554B02A630B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8745" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -657,43 +657,43 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1099,23 +1099,23 @@
   <dimension ref="B1:BO39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8:U9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.58203125" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="27" width="2.75" style="1"/>
     <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1125,14 +1125,14 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1140,37 +1140,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="30"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="31" t="s">
+      <c r="V2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="34"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="34"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
         <v>7</v>
@@ -1183,23 +1183,23 @@
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1225,13 +1225,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1">
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="24" t="s">
         <v>15</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="25" t="s">
         <v>16</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="25" t="s">
         <v>17</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="25" t="s">
         <v>18</v>
       </c>
@@ -1490,10 +1490,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="8">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="25" t="s">
         <v>19</v>
       </c>
@@ -1510,10 +1510,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="25" t="s">
         <v>20</v>
       </c>
@@ -1526,10 +1526,12 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="25" t="s">
         <v>21</v>
       </c>
@@ -1542,10 +1544,11 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="18"/>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="25" t="s">
         <v>22</v>
       </c>
@@ -1558,10 +1561,11 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1">
+        <v>0.8</v>
+      </c>
+      <c r="R12" s="18"/>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="25" t="s">
         <v>23</v>
       </c>
@@ -1574,10 +1578,11 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="18"/>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="25" t="s">
         <v>24</v>
       </c>
@@ -1590,10 +1595,11 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="R14" s="18"/>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="25" t="s">
         <v>25</v>
       </c>
@@ -1606,10 +1612,11 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1633,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6" t="s">
         <v>28</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1657,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="6" t="s">
         <v>30</v>
       </c>
@@ -1669,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="6" t="s">
         <v>31</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="6" t="s">
         <v>32</v>
       </c>
@@ -1693,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="6" t="s">
         <v>33</v>
       </c>
@@ -1705,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="6" t="s">
         <v>34</v>
       </c>
@@ -1717,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1729,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
         <v>36</v>
       </c>
@@ -1741,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="6" t="s">
         <v>37</v>
       </c>
@@ -1753,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="6" t="s">
         <v>38</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="6" t="s">
         <v>39</v>
       </c>
@@ -1777,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="6" t="s">
         <v>40</v>
       </c>
@@ -1789,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="6" t="s">
         <v>41</v>
       </c>
@@ -1801,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="6" t="s">
         <v>42</v>
       </c>
@@ -1813,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="6" t="s">
         <v>43</v>
       </c>
@@ -1825,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="6" t="s">
         <v>44</v>
       </c>
@@ -1837,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="6" t="s">
         <v>45</v>
       </c>
@@ -1849,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="6" t="s">
         <v>46</v>
       </c>
@@ -1861,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="6" t="s">
         <v>47</v>
       </c>
@@ -1873,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="6" t="s">
         <v>48</v>
       </c>
@@ -1885,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="6" t="s">
         <v>49</v>
       </c>
@@ -1899,19 +1906,19 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO39">
+  <conditionalFormatting sqref="H5:BO9 H16:BO39 H10:P10 H11:Q15 S10:BO15">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1948,8 +1955,8 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 Q10" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2 R10:R15" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>

</xml_diff>